<commit_message>
Changes in SCript with Merge sections
</commit_message>
<xml_diff>
--- a/R.P Smart Farming/2008.xlsx
+++ b/R.P Smart Farming/2008.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aman\Desktop\R.P Smart Farming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aman\Desktop\local_RP\R.P Smart Farming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B1F6B85-6364-40D3-8EE6-7FF6DEFE74DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD91BC0-6B17-4A5A-B1E1-A41279CA09DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E49030CF-C7A9-4901-89E1-B2536CF954FA}"/>
   </bookViews>
@@ -774,7 +774,7 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>

</xml_diff>